<commit_message>
Copy quotation.system to quotation.system_test_avivi
</commit_message>
<xml_diff>
--- a/local/components/custom/quotation.system_test_avivi/quatation_print.xlsx
+++ b/local/components/custom/quotation.system_test_avivi/quatation_print.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="105">
   <si>
     <t>METAL  PRO BUILDINGS</t>
   </si>
@@ -41,7 +41,7 @@
     <t>Customer ID:</t>
   </si>
   <si>
-    <t>L_53505</t>
+    <t>L_111343</t>
   </si>
   <si>
     <t xml:space="preserve">Customer : </t>
@@ -62,13 +62,10 @@
     <t>Email:</t>
   </si>
   <si>
-    <t>Nick Rojik</t>
+    <t>Kent  Chaulk</t>
   </si>
   <si>
-    <t>+1 8076318449</t>
-  </si>
-  <si>
-    <t>rojiknick@gmail.com</t>
+    <t>Inquire@live.ca</t>
   </si>
   <si>
     <t>Mailing Address:</t>
@@ -86,10 +83,10 @@
     <t>Building Address:</t>
   </si>
   <si>
-    <t>Thunder Bay</t>
+    <t>Labrador City</t>
   </si>
   <si>
-    <t>ON</t>
+    <t>NL</t>
   </si>
   <si>
     <t>Ship to:</t>
@@ -122,13 +119,16 @@
     <t>LOW (CATEGORY I) SHELTERED</t>
   </si>
   <si>
-    <t>ECONOSPAN</t>
+    <t>S-SERIES</t>
   </si>
   <si>
-    <t>Q30-14</t>
+    <t>S20-12</t>
   </si>
   <si>
     <t>TROUGH</t>
+  </si>
+  <si>
+    <t>22/20</t>
   </si>
   <si>
     <t xml:space="preserve">     Arches</t>
@@ -137,10 +137,10 @@
     <t xml:space="preserve">     Front Wall</t>
   </si>
   <si>
-    <t>FRAMED OPENING</t>
+    <t>OPEN</t>
   </si>
   <si>
-    <t>INCLUDED</t>
+    <t>LARGE C/A</t>
   </si>
   <si>
     <t>QTY</t>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>SOLID</t>
+  </si>
+  <si>
+    <t>INCLUDED</t>
   </si>
   <si>
     <t xml:space="preserve">     Accessories 
@@ -166,19 +169,13 @@
     <t>Height</t>
   </si>
   <si>
-    <t>Commercial Grade INSULATED Garage Doors</t>
-  </si>
-  <si>
-    <t>Service Door Insulated</t>
-  </si>
-  <si>
     <t>Insulation</t>
   </si>
   <si>
-    <t>Included</t>
+    <t>✔ 110% Nuts &amp; Bolts**</t>
   </si>
   <si>
-    <t>✔ 110% Nuts &amp; Bolts**</t>
+    <t>Not included</t>
   </si>
   <si>
     <t>✔30 Year Warranty**</t>
@@ -2385,11 +2382,11 @@
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
-      <c r="H8" s="27" t="s">
-        <v>16</v>
+      <c r="H8" s="27">
+        <v>17096972219</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J8" s="29"/>
       <c r="K8" s="30"/>
@@ -2411,21 +2408,21 @@
     </row>
     <row r="9" spans="1:28" customHeight="1" ht="30">
       <c r="A9" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="31"/>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
       <c r="E9" s="212" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="213"/>
       <c r="G9" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="214" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J9" s="215"/>
       <c r="K9" s="30"/>
@@ -2475,21 +2472,21 @@
     </row>
     <row r="11" spans="1:28" customHeight="1" ht="30">
       <c r="A11" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="33"/>
       <c r="E11" s="214" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="215"/>
       <c r="G11" s="214" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H11" s="215"/>
       <c r="I11" s="214" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J11" s="215"/>
       <c r="K11" s="16"/>
@@ -2515,11 +2512,11 @@
       <c r="C12" s="36"/>
       <c r="D12" s="37"/>
       <c r="E12" s="218" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="219"/>
       <c r="G12" s="34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H12" s="37"/>
       <c r="I12" s="34"/>
@@ -2571,21 +2568,21 @@
     </row>
     <row r="14" spans="1:28" customHeight="1" ht="30">
       <c r="A14" s="38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="D14" s="40"/>
       <c r="E14" s="222" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="223"/>
       <c r="G14" s="222" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H14" s="223"/>
       <c r="I14" s="222" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J14" s="223"/>
       <c r="K14" s="16"/>
@@ -2611,11 +2608,11 @@
       <c r="C15" s="36"/>
       <c r="D15" s="37"/>
       <c r="E15" s="218" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" s="219"/>
       <c r="G15" s="34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15" s="37"/>
       <c r="I15" s="34"/>
@@ -2667,30 +2664,30 @@
     </row>
     <row r="17" spans="1:28" customHeight="1" ht="35">
       <c r="A17" s="226" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="227"/>
       <c r="C17" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="E17" s="228" t="s">
         <v>28</v>
-      </c>
-      <c r="E17" s="228" t="s">
-        <v>29</v>
       </c>
       <c r="F17" s="229"/>
       <c r="G17" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="43" t="s">
+      <c r="I17" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="45" t="s">
+      <c r="J17" s="45" t="s">
         <v>32</v>
-      </c>
-      <c r="J17" s="45" t="s">
-        <v>33</v>
       </c>
       <c r="K17" s="46"/>
       <c r="L17" s="46"/>
@@ -2711,30 +2708,30 @@
     </row>
     <row r="18" spans="1:28" customHeight="1" ht="71.25">
       <c r="A18" s="230" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="231"/>
       <c r="C18" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="E18" s="47" t="s">
         <v>36</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>37</v>
       </c>
       <c r="F18" s="49"/>
       <c r="G18" s="50">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H18" s="51">
         <v>30</v>
       </c>
       <c r="I18" s="52">
-        <v>14</v>
+        <v>12</v>
       </c>
-      <c r="J18" s="52">
-        <v>22</v>
+      <c r="J18" s="52" t="s">
+        <v>37</v>
       </c>
       <c r="K18" s="53"/>
       <c r="L18" s="53"/>
@@ -2911,20 +2908,20 @@
         <v>42</v>
       </c>
       <c r="D24" s="67" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E24" s="67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F24" s="68"/>
       <c r="G24" s="69" t="s">
         <v>42</v>
       </c>
       <c r="H24" s="67" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I24" s="67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J24" s="70"/>
       <c r="K24" s="71"/>
@@ -2950,12 +2947,8 @@
       <c r="C25" s="48">
         <v>1</v>
       </c>
-      <c r="D25" s="73">
-        <v>10</v>
-      </c>
-      <c r="E25" s="74">
-        <v>12</v>
-      </c>
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
       <c r="F25" s="75"/>
       <c r="G25" s="76"/>
       <c r="H25" s="73"/>
@@ -2988,7 +2981,7 @@
       </c>
       <c r="D26" s="79"/>
       <c r="E26" s="245" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F26" s="246"/>
       <c r="G26" s="80"/>
@@ -3019,20 +3012,20 @@
         <v>42</v>
       </c>
       <c r="D27" s="67" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E27" s="67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F27" s="83"/>
       <c r="G27" s="69" t="s">
         <v>42</v>
       </c>
       <c r="H27" s="67" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I27" s="67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J27" s="84"/>
       <c r="K27" s="85"/>
@@ -3112,7 +3105,7 @@
     </row>
     <row r="30" spans="1:28" customHeight="1" ht="37.5">
       <c r="A30" s="249" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B30" s="250"/>
       <c r="C30" s="250"/>
@@ -3258,7 +3251,7 @@
     </row>
     <row r="35" spans="1:28" customHeight="1" ht="36">
       <c r="A35" s="252" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B35" s="250"/>
       <c r="C35" s="250"/>
@@ -3295,10 +3288,10 @@
         <v>42</v>
       </c>
       <c r="F36" s="109" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G36" s="44" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H36" s="110"/>
       <c r="I36" s="111"/>
@@ -3321,21 +3314,13 @@
       <c r="Z36" s="113"/>
     </row>
     <row r="37" spans="1:28" customHeight="1" ht="36.75">
-      <c r="A37" s="48" t="s">
-        <v>49</v>
-      </c>
+      <c r="A37" s="48"/>
       <c r="B37" s="76"/>
       <c r="C37" s="114"/>
       <c r="D37" s="114"/>
-      <c r="E37" s="109">
-        <v>1</v>
-      </c>
-      <c r="F37" s="109">
-        <v>10</v>
-      </c>
-      <c r="G37" s="115">
-        <v>12</v>
-      </c>
+      <c r="E37" s="109"/>
+      <c r="F37" s="109"/>
+      <c r="G37" s="115"/>
       <c r="H37" s="116"/>
       <c r="I37" s="117"/>
       <c r="J37" s="118"/>
@@ -3357,21 +3342,13 @@
       <c r="Z37" s="72"/>
     </row>
     <row r="38" spans="1:28" customHeight="1" ht="34">
-      <c r="A38" s="48" t="s">
-        <v>50</v>
-      </c>
+      <c r="A38" s="48"/>
       <c r="B38" s="76"/>
       <c r="C38" s="114"/>
       <c r="D38" s="114"/>
-      <c r="E38" s="109">
-        <v>1</v>
-      </c>
-      <c r="F38" s="109">
-        <v>32</v>
-      </c>
-      <c r="G38" s="115">
-        <v>84</v>
-      </c>
+      <c r="E38" s="109"/>
+      <c r="F38" s="109"/>
+      <c r="G38" s="115"/>
       <c r="H38" s="119"/>
       <c r="I38" s="120"/>
       <c r="J38" s="121"/>
@@ -3422,22 +3399,20 @@
     </row>
     <row r="40" spans="1:28" customHeight="1" ht="34.5">
       <c r="A40" s="127" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40" s="128"/>
       <c r="C40" s="128"/>
       <c r="D40" s="129"/>
-      <c r="E40" s="130" t="s">
-        <v>52</v>
-      </c>
+      <c r="E40" s="130"/>
       <c r="F40" s="131" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G40" s="132"/>
       <c r="H40" s="133"/>
       <c r="I40" s="133"/>
       <c r="J40" s="134" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="K40" s="107"/>
       <c r="L40" s="107"/>
@@ -3461,15 +3436,17 @@
       <c r="B41" s="55"/>
       <c r="C41" s="135"/>
       <c r="D41" s="135"/>
-      <c r="E41" s="136"/>
+      <c r="E41" s="136" t="s">
+        <v>52</v>
+      </c>
       <c r="F41" s="137" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G41" s="138"/>
       <c r="H41" s="139"/>
       <c r="I41" s="139"/>
       <c r="J41" s="140" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="K41" s="72"/>
       <c r="L41" s="72"/>
@@ -3490,20 +3467,20 @@
     </row>
     <row r="42" spans="1:28" customHeight="1" ht="45">
       <c r="A42" s="141" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B42" s="142"/>
       <c r="C42" s="143"/>
       <c r="D42" s="144"/>
       <c r="E42" s="145"/>
       <c r="F42" s="146" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G42" s="146"/>
       <c r="H42" s="147"/>
       <c r="I42" s="147"/>
       <c r="J42" s="148" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="K42" s="149"/>
       <c r="L42" s="149"/>
@@ -3552,14 +3529,14 @@
     </row>
     <row r="44" spans="1:28" customHeight="1" ht="68.25">
       <c r="A44" s="150" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44" s="151"/>
       <c r="C44" s="152"/>
       <c r="D44" s="152"/>
       <c r="E44" s="153"/>
       <c r="F44" s="253" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G44" s="254"/>
       <c r="H44" s="254"/>
@@ -3584,13 +3561,13 @@
     </row>
     <row r="45" spans="1:28" customHeight="1" ht="35.25">
       <c r="A45" s="154" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B45" s="155"/>
       <c r="C45" s="156"/>
       <c r="D45" s="156"/>
       <c r="E45" s="157" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F45" s="225"/>
       <c r="G45" s="225"/>
@@ -3734,13 +3711,11 @@
       <c r="E50" s="169"/>
       <c r="F50" s="169"/>
       <c r="G50" s="204" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H50" s="205"/>
       <c r="I50" s="205"/>
-      <c r="J50" s="170">
-        <v>18233.1992</v>
-      </c>
+      <c r="J50" s="170"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
@@ -3766,12 +3741,12 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
       <c r="G51" s="209" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H51" s="210"/>
       <c r="I51" s="211"/>
       <c r="J51" s="172">
-        <v>590</v>
+        <v>21698.496923077</v>
       </c>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
@@ -3798,12 +3773,12 @@
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
       <c r="G52" s="206" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H52" s="207"/>
       <c r="I52" s="208"/>
       <c r="J52" s="173">
-        <v>18823.1992</v>
+        <v>6000.0</v>
       </c>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
@@ -3832,7 +3807,9 @@
       <c r="G53" s="177"/>
       <c r="H53" s="177"/>
       <c r="I53" s="178"/>
-      <c r="J53" s="179"/>
+      <c r="J53" s="179">
+        <v>27698.496923077</v>
+      </c>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
@@ -3936,18 +3913,18 @@
     </row>
     <row r="57" spans="1:28" customHeight="1" ht="26.25">
       <c r="A57" s="186" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B57" s="180"/>
       <c r="C57" s="66" t="str">
         <f>$A$8&amp;" "&amp;$E$8</f>
-        <v>Nick Rojik </v>
+        <v>Kent  Chaulk </v>
       </c>
       <c r="D57" s="181"/>
       <c r="E57" s="181"/>
       <c r="F57" s="181"/>
       <c r="G57" s="187" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H57" s="180"/>
       <c r="I57" s="182"/>
@@ -3977,7 +3954,7 @@
       <c r="E58" s="181"/>
       <c r="F58" s="181"/>
       <c r="G58" s="184" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H58" s="180"/>
       <c r="I58" s="182"/>
@@ -4141,13 +4118,13 @@
     </row>
     <row r="64" spans="1:28" customHeight="1" ht="15.75">
       <c r="A64" s="193" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -4201,7 +4178,7 @@
     </row>
     <row r="66" spans="1:28" customHeight="1" ht="63">
       <c r="A66" s="260" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66" s="261"/>
       <c r="C66" s="261"/>
@@ -4231,7 +4208,7 @@
     </row>
     <row r="67" spans="1:28" customHeight="1" ht="33">
       <c r="A67" s="263" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B67" s="264"/>
       <c r="C67" s="264"/>
@@ -4261,7 +4238,7 @@
     </row>
     <row r="68" spans="1:28" customHeight="1" ht="32">
       <c r="A68" s="263" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B68" s="264"/>
       <c r="C68" s="264"/>
@@ -4291,7 +4268,7 @@
     </row>
     <row r="69" spans="1:28" customHeight="1" ht="48">
       <c r="A69" s="263" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B69" s="264"/>
       <c r="C69" s="264"/>
@@ -4321,7 +4298,7 @@
     </row>
     <row r="70" spans="1:28" customHeight="1" ht="30">
       <c r="A70" s="266" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B70" s="267"/>
       <c r="C70" s="267"/>
@@ -4351,7 +4328,7 @@
     </row>
     <row r="71" spans="1:28" customHeight="1" ht="66">
       <c r="A71" s="266" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B71" s="267"/>
       <c r="C71" s="267"/>
@@ -4381,7 +4358,7 @@
     </row>
     <row r="72" spans="1:28" customHeight="1" ht="64">
       <c r="A72" s="266" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B72" s="267"/>
       <c r="C72" s="267"/>
@@ -4411,7 +4388,7 @@
     </row>
     <row r="73" spans="1:28" customHeight="1" ht="30">
       <c r="A73" s="266" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B73" s="267"/>
       <c r="C73" s="267"/>
@@ -4441,7 +4418,7 @@
     </row>
     <row r="74" spans="1:28" customHeight="1" ht="18">
       <c r="A74" s="266" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B74" s="267"/>
       <c r="C74" s="267"/>
@@ -4471,7 +4448,7 @@
     </row>
     <row r="75" spans="1:28" customHeight="1" ht="33">
       <c r="A75" s="266" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B75" s="267"/>
       <c r="C75" s="267"/>
@@ -4501,7 +4478,7 @@
     </row>
     <row r="76" spans="1:28" customHeight="1" ht="31">
       <c r="A76" s="266" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B76" s="267"/>
       <c r="C76" s="267"/>
@@ -4531,7 +4508,7 @@
     </row>
     <row r="77" spans="1:28" customHeight="1" ht="18">
       <c r="A77" s="266" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B77" s="267"/>
       <c r="C77" s="267"/>
@@ -4561,7 +4538,7 @@
     </row>
     <row r="78" spans="1:28" customHeight="1" ht="17">
       <c r="A78" s="266" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78" s="267"/>
       <c r="C78" s="267"/>
@@ -4591,7 +4568,7 @@
     </row>
     <row r="79" spans="1:28" customHeight="1" ht="32">
       <c r="A79" s="266" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B79" s="267"/>
       <c r="C79" s="267"/>
@@ -4621,7 +4598,7 @@
     </row>
     <row r="80" spans="1:28" customHeight="1" ht="48">
       <c r="A80" s="266" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B80" s="267"/>
       <c r="C80" s="267"/>
@@ -4651,7 +4628,7 @@
     </row>
     <row r="81" spans="1:28" customHeight="1" ht="17">
       <c r="A81" s="266" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B81" s="267"/>
       <c r="C81" s="267"/>
@@ -4681,7 +4658,7 @@
     </row>
     <row r="82" spans="1:28" customHeight="1" ht="50">
       <c r="A82" s="266" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B82" s="267"/>
       <c r="C82" s="267"/>
@@ -4711,7 +4688,7 @@
     </row>
     <row r="83" spans="1:28" customHeight="1" ht="17">
       <c r="A83" s="266" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B83" s="267"/>
       <c r="C83" s="267"/>
@@ -4741,7 +4718,7 @@
     </row>
     <row r="84" spans="1:28" customHeight="1" ht="32">
       <c r="A84" s="266" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B84" s="267"/>
       <c r="C84" s="267"/>
@@ -4771,7 +4748,7 @@
     </row>
     <row r="85" spans="1:28" customHeight="1" ht="32">
       <c r="A85" s="266" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B85" s="267"/>
       <c r="C85" s="267"/>
@@ -4801,7 +4778,7 @@
     </row>
     <row r="86" spans="1:28" customHeight="1" ht="23">
       <c r="A86" s="266" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B86" s="267"/>
       <c r="C86" s="267"/>
@@ -4831,7 +4808,7 @@
     </row>
     <row r="87" spans="1:28" customHeight="1" ht="17">
       <c r="A87" s="266" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B87" s="267"/>
       <c r="C87" s="267"/>
@@ -4861,7 +4838,7 @@
     </row>
     <row r="88" spans="1:28" customHeight="1" ht="16" s="201" customFormat="1">
       <c r="A88" s="266" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B88" s="267"/>
       <c r="C88" s="267"/>
@@ -4891,7 +4868,7 @@
     </row>
     <row r="89" spans="1:28" customHeight="1" ht="19">
       <c r="A89" s="266" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B89" s="267"/>
       <c r="C89" s="267"/>
@@ -4921,7 +4898,7 @@
     </row>
     <row r="90" spans="1:28" customHeight="1" ht="18">
       <c r="A90" s="266" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B90" s="267"/>
       <c r="C90" s="267"/>
@@ -4951,7 +4928,7 @@
     </row>
     <row r="91" spans="1:28" customHeight="1" ht="31">
       <c r="A91" s="266" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B91" s="267"/>
       <c r="C91" s="267"/>
@@ -4981,7 +4958,7 @@
     </row>
     <row r="92" spans="1:28" customHeight="1" ht="34.5">
       <c r="A92" s="266" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B92" s="267"/>
       <c r="C92" s="267"/>
@@ -5011,7 +4988,7 @@
     </row>
     <row r="93" spans="1:28" customHeight="1" ht="31">
       <c r="A93" s="266" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B93" s="267"/>
       <c r="C93" s="267"/>
@@ -5041,7 +5018,7 @@
     </row>
     <row r="94" spans="1:28" customHeight="1" ht="32">
       <c r="A94" s="266" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B94" s="267"/>
       <c r="C94" s="267"/>
@@ -5071,7 +5048,7 @@
     </row>
     <row r="95" spans="1:28" customHeight="1" ht="18">
       <c r="A95" s="266" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B95" s="267"/>
       <c r="C95" s="267"/>
@@ -5101,7 +5078,7 @@
     </row>
     <row r="96" spans="1:28" customHeight="1" ht="51">
       <c r="A96" s="266" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B96" s="267"/>
       <c r="C96" s="267"/>
@@ -5131,7 +5108,7 @@
     </row>
     <row r="97" spans="1:28" customHeight="1" ht="18">
       <c r="A97" s="266" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B97" s="267"/>
       <c r="C97" s="267"/>
@@ -5161,7 +5138,7 @@
     </row>
     <row r="98" spans="1:28" customHeight="1" ht="33">
       <c r="A98" s="266" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B98" s="267"/>
       <c r="C98" s="267"/>
@@ -5191,7 +5168,7 @@
     </row>
     <row r="99" spans="1:28" customHeight="1" ht="33">
       <c r="A99" s="266" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B99" s="267"/>
       <c r="C99" s="267"/>
@@ -5221,7 +5198,7 @@
     </row>
     <row r="100" spans="1:28" customHeight="1" ht="35">
       <c r="A100" s="266" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B100" s="267"/>
       <c r="C100" s="267"/>
@@ -5251,7 +5228,7 @@
     </row>
     <row r="101" spans="1:28" customHeight="1" ht="46">
       <c r="A101" s="274" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B101" s="267"/>
       <c r="C101" s="267"/>
@@ -5281,7 +5258,7 @@
     </row>
     <row r="102" spans="1:28" customHeight="1" ht="26" s="201" customFormat="1">
       <c r="A102" s="271" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B102" s="271"/>
       <c r="C102" s="271"/>

</xml_diff>